<commit_message>
recent changes for CI/CD
</commit_message>
<xml_diff>
--- a/src/test/resources/BlankData.xlsx
+++ b/src/test/resources/BlankData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="265">
   <si>
     <t>USERNAME</t>
   </si>
@@ -623,6 +623,201 @@
   </si>
   <si>
     <t>SC1478922</t>
+  </si>
+  <si>
+    <t>dmech+ruan@barcodesinc.com</t>
+  </si>
+  <si>
+    <t>SC1653514</t>
+  </si>
+  <si>
+    <t>SC1648828</t>
+  </si>
+  <si>
+    <t>SC1633603</t>
+  </si>
+  <si>
+    <t>SC1630499</t>
+  </si>
+  <si>
+    <t>SC1623968</t>
+  </si>
+  <si>
+    <t>SC1623569</t>
+  </si>
+  <si>
+    <t>SC1623546</t>
+  </si>
+  <si>
+    <t>SC1623520</t>
+  </si>
+  <si>
+    <t>SC1582517</t>
+  </si>
+  <si>
+    <t>SC1512216</t>
+  </si>
+  <si>
+    <t>SC1511875</t>
+  </si>
+  <si>
+    <t>dmech+newhudson@barcodesinc.com</t>
+  </si>
+  <si>
+    <t>dmech+worley@barcodesinc.com</t>
+  </si>
+  <si>
+    <t>SC1656080</t>
+  </si>
+  <si>
+    <t>SC1654961</t>
+  </si>
+  <si>
+    <t>SC1649544</t>
+  </si>
+  <si>
+    <t>SC1648326</t>
+  </si>
+  <si>
+    <t>SC1642676</t>
+  </si>
+  <si>
+    <t>SC1635861</t>
+  </si>
+  <si>
+    <t>SC1628787</t>
+  </si>
+  <si>
+    <t>SC1624090</t>
+  </si>
+  <si>
+    <t>SC1596139</t>
+  </si>
+  <si>
+    <t>SC1594809</t>
+  </si>
+  <si>
+    <t>SC1589898</t>
+  </si>
+  <si>
+    <t>SC1584776</t>
+  </si>
+  <si>
+    <t>dmech+rakuten2@barcodesinc.com</t>
+  </si>
+  <si>
+    <t>SC1637414</t>
+  </si>
+  <si>
+    <t>SC1625170</t>
+  </si>
+  <si>
+    <t>SC1616618</t>
+  </si>
+  <si>
+    <t>dmech+penske@barcodesinc.com</t>
+  </si>
+  <si>
+    <t>SC1527193</t>
+  </si>
+  <si>
+    <t>SC1656993</t>
+  </si>
+  <si>
+    <t>dmech+greco@barcodesinc.com</t>
+  </si>
+  <si>
+    <t>SC1659465</t>
+  </si>
+  <si>
+    <t>SC1655543</t>
+  </si>
+  <si>
+    <t>SC1648899</t>
+  </si>
+  <si>
+    <t>SC1625129</t>
+  </si>
+  <si>
+    <t>SC1625041</t>
+  </si>
+  <si>
+    <t>SC1619781</t>
+  </si>
+  <si>
+    <t>SC1614845</t>
+  </si>
+  <si>
+    <t>SC1614740</t>
+  </si>
+  <si>
+    <t>SC1607016</t>
+  </si>
+  <si>
+    <t>SC1589419</t>
+  </si>
+  <si>
+    <t>ID1858-11</t>
+  </si>
+  <si>
+    <t>ID1858-10</t>
+  </si>
+  <si>
+    <t>ID1858-9</t>
+  </si>
+  <si>
+    <t>ID1858-7</t>
+  </si>
+  <si>
+    <t>ID1858-8</t>
+  </si>
+  <si>
+    <t>ID1858-6</t>
+  </si>
+  <si>
+    <t>ID1858-4</t>
+  </si>
+  <si>
+    <t>ID1858-5</t>
+  </si>
+  <si>
+    <t>ID1858-3</t>
+  </si>
+  <si>
+    <t>ID1858-1</t>
+  </si>
+  <si>
+    <t>ID1858-2</t>
+  </si>
+  <si>
+    <t>ID1859-7</t>
+  </si>
+  <si>
+    <t>ID1859-4</t>
+  </si>
+  <si>
+    <t>ID1859-5</t>
+  </si>
+  <si>
+    <t>ID1859-6</t>
+  </si>
+  <si>
+    <t>ID1859-2</t>
+  </si>
+  <si>
+    <t>SC1537274</t>
+  </si>
+  <si>
+    <t>SC1530937</t>
+  </si>
+  <si>
+    <t>SC1520339</t>
+  </si>
+  <si>
+    <t>SC1482696</t>
+  </si>
+  <si>
+    <t>SC1482694</t>
   </si>
 </sst>
 </file>
@@ -659,7 +854,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="238">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1132,30 +1399,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="163">
+      <c r="A1" t="s" s="235">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="164">
+      <c r="B1" t="s" s="236">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="165">
+      <c r="C1" t="s" s="237">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>76</v>
+        <v>234</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1163,7 +1430,7 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>235</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -1171,7 +1438,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1179,48 +1446,297 @@
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>79</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>260</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>260</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>261</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>262</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>263</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>264</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="43"/>
     <row r="44"/>
     <row r="45"/>

</xml_diff>